<commit_message>
Version 1.1.0 with updated emission factor inputs and emission outputs
- This release of PIER is compatible with v1.1.0 of Rumi which has
  emissions post-processing implmentation
- Emission factor inputs have been updated based on literature, and
  these are used to calculate emissions for all scenarios and
  sensitivity runs
- Minor fix: a superfluous column LIGHT_ELEC_ES_Demand.csv has been
  removed
</commit_message>
<xml_diff>
--- a/Docs/Parameters & Source file-map.xlsx
+++ b/Docs/Parameters & Source file-map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prayas\EnMo\Rumi-India\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prayas\EnMo\Git\Rumi-India\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="FileInfo" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="166">
   <si>
     <t>CurrencyUnit.csv</t>
   </si>
@@ -546,6 +546,15 @@
   </si>
   <si>
     <t>ST_Efficiency_EfficiencyLevelSplit.xlsx</t>
+  </si>
+  <si>
+    <t>ST_EmissionDetails.csv</t>
+  </si>
+  <si>
+    <t>ECT_EmissionDetails.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emission_Factors.xlsx </t>
   </si>
 </sst>
 </file>
@@ -867,6 +876,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,9 +893,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,77 +1266,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2021</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="35">
-        <v>44470</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
+      <c r="B4" s="38">
+        <v>44651</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -1341,15 +1350,15 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -1359,15 +1368,15 @@
       <c r="B8" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1377,13 +1386,13 @@
       <c r="B9" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1393,15 +1402,15 @@
       <c r="B10" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -4336,13 +4345,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4470,10 +4479,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -4496,7 +4505,7 @@
         <v>147</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -4519,7 +4528,7 @@
         <v>147</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -4542,7 +4551,7 @@
         <v>147</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -4565,7 +4574,7 @@
         <v>147</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -4588,24 +4597,16 @@
         <v>147</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -4619,7 +4620,7 @@
         <v>147</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -4650,7 +4651,7 @@
         <v>147</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -4662,8 +4663,12 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -4677,7 +4682,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -4704,14 +4709,18 @@
         <v>147</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -4727,7 +4736,7 @@
         <v>147</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -4750,7 +4759,7 @@
         <v>147</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -4770,10 +4779,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -4796,26 +4805,18 @@
         <v>148</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -4827,24 +4828,28 @@
         <v>148</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -4854,7 +4859,7 @@
         <v>148</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -4866,8 +4871,12 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -4877,7 +4886,7 @@
         <v>148</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -4900,7 +4909,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -4923,7 +4932,7 @@
         <v>148</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -4946,7 +4955,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -4960,12 +4969,8 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3">
-        <v>1</v>
-      </c>
-      <c r="N24" s="3">
-        <v>1</v>
-      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -4973,7 +4978,7 @@
         <v>148</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -4987,15 +4992,20 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="M25" s="3">
+        <v>1</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+      <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -5011,14 +5021,13 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -5037,11 +5046,11 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>129</v>
+      <c r="B28" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -5059,8 +5068,31 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C7 C9:C28">
+  <conditionalFormatting sqref="C10:C29 C2:C8">
     <cfRule type="iconSet" priority="9">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5069,7 +5101,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C9">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5078,7 +5110,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:O8">
+  <conditionalFormatting sqref="D9:O9">
     <cfRule type="iconSet" priority="13">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5087,7 +5119,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:O7 D9:O24 D26:O28 D25:N25">
+  <conditionalFormatting sqref="D2:O8 D10:O25 D27:O29 D26:N26">
     <cfRule type="iconSet" priority="14">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5103,7 +5135,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -5941,21 +5973,17 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="C35" s="19">
         <v>1</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="3">
-        <v>1</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -5971,14 +5999,18 @@
         <v>136</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="19">
         <v>1</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -5994,18 +6026,14 @@
         <v>136</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="19">
         <v>1</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="3">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1</v>
-      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -6021,14 +6049,18 @@
         <v>136</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="19">
         <v>1</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -6044,18 +6076,14 @@
         <v>136</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="19">
         <v>1</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="3">
-        <v>1</v>
-      </c>
-      <c r="F39" s="3">
-        <v>1</v>
-      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -6064,16 +6092,14 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="3">
-        <v>1</v>
-      </c>
+      <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="19">
         <v>1</v>
@@ -6093,21 +6119,27 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="O40" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="19">
         <v>1</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -6123,18 +6155,14 @@
         <v>136</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="19">
         <v>1</v>
       </c>
       <c r="D42" s="3"/>
-      <c r="E42" s="3">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1</v>
-      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -6150,14 +6178,18 @@
         <v>136</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="19">
         <v>1</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -6173,7 +6205,7 @@
         <v>136</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" s="19">
         <v>1</v>
@@ -6196,18 +6228,14 @@
         <v>136</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="19">
         <v>1</v>
       </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="3">
-        <v>1</v>
-      </c>
-      <c r="F45" s="3">
-        <v>1</v>
-      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -6223,14 +6251,18 @@
         <v>136</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="19">
         <v>1</v>
       </c>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -6243,27 +6275,19 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="19">
         <v>1</v>
       </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3">
-        <v>1</v>
-      </c>
-      <c r="H47" s="3">
-        <v>1</v>
-      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -6277,7 +6301,7 @@
         <v>137</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="19">
         <v>1</v>
@@ -6308,7 +6332,7 @@
         <v>137</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C49" s="19">
         <v>1</v>
@@ -6320,24 +6344,26 @@
       <c r="F49" s="3">
         <v>1</v>
       </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="G49" s="3">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <v>1</v>
+      </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="3">
-        <v>1</v>
-      </c>
+      <c r="O49" s="3"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C50" s="19">
         <v>1</v>
@@ -6357,14 +6383,16 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
+      <c r="O50" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="19">
         <v>1</v>
@@ -6391,7 +6419,7 @@
         <v>137</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C52" s="19">
         <v>1</v>
@@ -6418,7 +6446,7 @@
         <v>137</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C53" s="19">
         <v>1</v>
@@ -6430,12 +6458,8 @@
       <c r="F53" s="3">
         <v>1</v>
       </c>
-      <c r="G53" s="3">
-        <v>1</v>
-      </c>
-      <c r="H53" s="3">
-        <v>1</v>
-      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -6449,7 +6473,7 @@
         <v>137</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C54" s="19">
         <v>1</v>
@@ -6461,8 +6485,12 @@
       <c r="F54" s="3">
         <v>1</v>
       </c>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
+      <c r="G54" s="3">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -6473,10 +6501,10 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C55" s="19">
         <v>1</v>
@@ -6496,16 +6524,14 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
-      <c r="O55" s="3">
-        <v>1</v>
-      </c>
+      <c r="O55" s="3"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C56" s="19">
         <v>1</v>
@@ -6525,21 +6551,27 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
+      <c r="O56" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C57" s="19">
         <v>1</v>
       </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -6555,18 +6587,14 @@
         <v>138</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C58" s="19">
         <v>1</v>
       </c>
       <c r="D58" s="3"/>
-      <c r="E58" s="3">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1</v>
-      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -6579,10 +6607,10 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C59" s="19">
         <v>1</v>
@@ -6602,16 +6630,14 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
-      <c r="O59" s="3">
-        <v>1</v>
-      </c>
+      <c r="O59" s="3"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C60" s="19">
         <v>1</v>
@@ -6631,21 +6657,27 @@
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
+      <c r="O60" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C61" s="19">
         <v>1</v>
       </c>
       <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1</v>
+      </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -6661,7 +6693,7 @@
         <v>139</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C62" s="19">
         <v>1</v>
@@ -6681,10 +6713,10 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C63" s="19">
         <v>1</v>
@@ -6707,7 +6739,7 @@
         <v>140</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C64" s="19">
         <v>1</v>
@@ -6730,18 +6762,14 @@
         <v>140</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C65" s="19">
         <v>1</v>
       </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="3">
-        <v>1</v>
-      </c>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -6754,17 +6782,21 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C66" s="19">
         <v>1</v>
       </c>
       <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
+      <c r="E66" s="3">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -6780,7 +6812,7 @@
         <v>141</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C67" s="19">
         <v>1</v>
@@ -6803,7 +6835,7 @@
         <v>141</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C68" s="19">
         <v>1</v>
@@ -6826,7 +6858,7 @@
         <v>141</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C69" s="19">
         <v>1</v>
@@ -6849,7 +6881,7 @@
         <v>141</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C70" s="19">
         <v>1</v>
@@ -6872,7 +6904,7 @@
         <v>141</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C71" s="19">
         <v>1</v>
@@ -6892,10 +6924,10 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C72" s="19">
         <v>1</v>
@@ -6918,7 +6950,7 @@
         <v>142</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C73" s="19">
         <v>1</v>
@@ -6930,12 +6962,8 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="3">
-        <v>1</v>
-      </c>
-      <c r="L73" s="3">
-        <v>1</v>
-      </c>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
@@ -6945,7 +6973,7 @@
         <v>142</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C74" s="19">
         <v>1</v>
@@ -6957,18 +6985,22 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
+      <c r="K74" s="3">
+        <v>1</v>
+      </c>
+      <c r="L74" s="3">
+        <v>1</v>
+      </c>
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C75" s="19">
         <v>1</v>
@@ -6991,18 +7023,14 @@
         <v>143</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C76" s="19">
         <v>1</v>
       </c>
       <c r="D76" s="3"/>
-      <c r="E76" s="3">
-        <v>1</v>
-      </c>
-      <c r="F76" s="3">
-        <v>1</v>
-      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -7018,14 +7046,18 @@
         <v>143</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" s="19">
         <v>1</v>
       </c>
       <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1</v>
+      </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -7041,7 +7073,7 @@
         <v>143</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C78" s="19">
         <v>1</v>
@@ -7055,12 +7087,8 @@
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
-      <c r="M78" s="3">
-        <v>1</v>
-      </c>
-      <c r="N78" s="3">
-        <v>1</v>
-      </c>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
       <c r="O78" s="3"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -7068,7 +7096,7 @@
         <v>143</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="19">
         <v>1</v>
@@ -7082,8 +7110,12 @@
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
+      <c r="M79" s="3">
+        <v>1</v>
+      </c>
+      <c r="N79" s="3">
+        <v>1</v>
+      </c>
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -7091,7 +7123,7 @@
         <v>143</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="19">
         <v>1</v>
@@ -7111,29 +7143,21 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C81" s="19">
         <v>1</v>
       </c>
       <c r="D81" s="3"/>
-      <c r="E81" s="3">
-        <v>1</v>
-      </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="3">
-        <v>1</v>
-      </c>
-      <c r="J81" s="3">
-        <v>1</v>
-      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
@@ -7145,7 +7169,7 @@
         <v>144</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C82" s="19">
         <v>1</v>
@@ -7154,17 +7178,19 @@
       <c r="E82" s="3">
         <v>1</v>
       </c>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3">
-        <v>1</v>
-      </c>
-      <c r="L82" s="3">
-        <v>1</v>
-      </c>
+      <c r="I82" s="3">
+        <v>1</v>
+      </c>
+      <c r="J82" s="3">
+        <v>1</v>
+      </c>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
@@ -7174,20 +7200,26 @@
         <v>144</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C83" s="19">
         <v>1</v>
       </c>
       <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+      <c r="E83" s="3">
+        <v>1</v>
+      </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
+      <c r="K83" s="3">
+        <v>1</v>
+      </c>
+      <c r="L83" s="3">
+        <v>1</v>
+      </c>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
@@ -7197,15 +7229,13 @@
         <v>144</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C84" s="19">
         <v>1</v>
       </c>
       <c r="D84" s="3"/>
-      <c r="E84" s="3">
-        <v>1</v>
-      </c>
+      <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -7222,13 +7252,15 @@
         <v>144</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C85" s="19">
         <v>1</v>
       </c>
       <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3">
+        <v>1</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -7245,7 +7277,7 @@
         <v>144</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C86" s="19">
         <v>1</v>
@@ -7268,15 +7300,13 @@
         <v>144</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" s="19">
         <v>1</v>
       </c>
       <c r="D87" s="3"/>
-      <c r="E87" s="3">
-        <v>1</v>
-      </c>
+      <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -7293,13 +7323,15 @@
         <v>144</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C88" s="19">
         <v>1</v>
       </c>
       <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
+      <c r="E88" s="3">
+        <v>1</v>
+      </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -7312,22 +7344,18 @@
       <c r="O88" s="3"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B89" s="24" t="s">
-        <v>76</v>
+      <c r="A89" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B89" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="C89" s="19">
         <v>1</v>
       </c>
       <c r="D89" s="3"/>
-      <c r="E89" s="3">
-        <v>1</v>
-      </c>
-      <c r="F89" s="3">
-        <v>1</v>
-      </c>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -7337,6 +7365,56 @@
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
       <c r="O89" s="3"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C90" s="19">
+        <v>1</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C91" s="19">
+        <v>1</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>1</v>
+      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C21:C22 C2:C19">
@@ -7348,7 +7426,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C89">
+  <conditionalFormatting sqref="C3:C91">
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -7375,7 +7453,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:O89">
+  <conditionalFormatting sqref="D3:O91">
     <cfRule type="iconSet" priority="17">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
Updated emission factor inputs and emission outputs
- This release of PIER is compatible with v1.1.0 of Rumi which has
  emissions post-processing implmentation
- Emission factor inputs have been updated based on literature, and
  these are used to calculate emissions for all scenarios and
  sensitivity runs
- Minor fix: a superfluous column LIGHT_ELEC_ES_Demand.csv has been
  removed
</commit_message>
<xml_diff>
--- a/Docs/Parameters & Source file-map.xlsx
+++ b/Docs/Parameters & Source file-map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prayas\EnMo\Rumi-India\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prayas\EnMo\Git\Rumi-India\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="FileInfo" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="166">
   <si>
     <t>CurrencyUnit.csv</t>
   </si>
@@ -546,6 +546,15 @@
   </si>
   <si>
     <t>ST_Efficiency_EfficiencyLevelSplit.xlsx</t>
+  </si>
+  <si>
+    <t>ST_EmissionDetails.csv</t>
+  </si>
+  <si>
+    <t>ECT_EmissionDetails.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emission_Factors.xlsx </t>
   </si>
 </sst>
 </file>
@@ -867,6 +876,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,9 +893,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,77 +1266,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2021</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="35">
-        <v>44470</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
+      <c r="B4" s="38">
+        <v>44651</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -1341,15 +1350,15 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -1359,15 +1368,15 @@
       <c r="B8" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1377,13 +1386,13 @@
       <c r="B9" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1393,15 +1402,15 @@
       <c r="B10" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
@@ -4336,13 +4345,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4470,10 +4479,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -4496,7 +4505,7 @@
         <v>147</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -4519,7 +4528,7 @@
         <v>147</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -4542,7 +4551,7 @@
         <v>147</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -4565,7 +4574,7 @@
         <v>147</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -4588,24 +4597,16 @@
         <v>147</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -4619,7 +4620,7 @@
         <v>147</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -4650,7 +4651,7 @@
         <v>147</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -4662,8 +4663,12 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -4677,7 +4682,7 @@
         <v>147</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -4704,14 +4709,18 @@
         <v>147</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -4727,7 +4736,7 @@
         <v>147</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -4750,7 +4759,7 @@
         <v>147</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -4770,10 +4779,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -4796,26 +4805,18 @@
         <v>148</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3">
-        <v>1</v>
-      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -4827,24 +4828,28 @@
         <v>148</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -4854,7 +4859,7 @@
         <v>148</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -4866,8 +4871,12 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -4877,7 +4886,7 @@
         <v>148</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -4900,7 +4909,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -4923,7 +4932,7 @@
         <v>148</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -4946,7 +4955,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -4960,12 +4969,8 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3">
-        <v>1</v>
-      </c>
-      <c r="N24" s="3">
-        <v>1</v>
-      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -4973,7 +4978,7 @@
         <v>148</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -4987,15 +4992,20 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="M25" s="3">
+        <v>1</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+      <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -5011,14 +5021,13 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -5037,11 +5046,11 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>129</v>
+      <c r="B28" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -5059,8 +5068,31 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C7 C9:C28">
+  <conditionalFormatting sqref="C10:C29 C2:C8">
     <cfRule type="iconSet" priority="9">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5069,7 +5101,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C9">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5078,7 +5110,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:O8">
+  <conditionalFormatting sqref="D9:O9">
     <cfRule type="iconSet" priority="13">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5087,7 +5119,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:O7 D9:O24 D26:O28 D25:N25">
+  <conditionalFormatting sqref="D2:O8 D10:O25 D27:O29 D26:N26">
     <cfRule type="iconSet" priority="14">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -5103,7 +5135,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -5941,21 +5973,17 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="C35" s="19">
         <v>1</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="3">
-        <v>1</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -5971,14 +5999,18 @@
         <v>136</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="19">
         <v>1</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -5994,18 +6026,14 @@
         <v>136</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="19">
         <v>1</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="3">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1</v>
-      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -6021,14 +6049,18 @@
         <v>136</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="19">
         <v>1</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -6044,18 +6076,14 @@
         <v>136</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="19">
         <v>1</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="3">
-        <v>1</v>
-      </c>
-      <c r="F39" s="3">
-        <v>1</v>
-      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -6064,16 +6092,14 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="3">
-        <v>1</v>
-      </c>
+      <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="19">
         <v>1</v>
@@ -6093,21 +6119,27 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="O40" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="19">
         <v>1</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -6123,18 +6155,14 @@
         <v>136</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="19">
         <v>1</v>
       </c>
       <c r="D42" s="3"/>
-      <c r="E42" s="3">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1</v>
-      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -6150,14 +6178,18 @@
         <v>136</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" s="19">
         <v>1</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -6173,7 +6205,7 @@
         <v>136</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" s="19">
         <v>1</v>
@@ -6196,18 +6228,14 @@
         <v>136</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="19">
         <v>1</v>
       </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="3">
-        <v>1</v>
-      </c>
-      <c r="F45" s="3">
-        <v>1</v>
-      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -6223,14 +6251,18 @@
         <v>136</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="19">
         <v>1</v>
       </c>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -6243,27 +6275,19 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="19">
         <v>1</v>
       </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3">
-        <v>1</v>
-      </c>
-      <c r="H47" s="3">
-        <v>1</v>
-      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -6277,7 +6301,7 @@
         <v>137</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" s="19">
         <v>1</v>
@@ -6308,7 +6332,7 @@
         <v>137</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C49" s="19">
         <v>1</v>
@@ -6320,24 +6344,26 @@
       <c r="F49" s="3">
         <v>1</v>
       </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="G49" s="3">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <v>1</v>
+      </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="3">
-        <v>1</v>
-      </c>
+      <c r="O49" s="3"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C50" s="19">
         <v>1</v>
@@ -6357,14 +6383,16 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
+      <c r="O50" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="19">
         <v>1</v>
@@ -6391,7 +6419,7 @@
         <v>137</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C52" s="19">
         <v>1</v>
@@ -6418,7 +6446,7 @@
         <v>137</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C53" s="19">
         <v>1</v>
@@ -6430,12 +6458,8 @@
       <c r="F53" s="3">
         <v>1</v>
       </c>
-      <c r="G53" s="3">
-        <v>1</v>
-      </c>
-      <c r="H53" s="3">
-        <v>1</v>
-      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -6449,7 +6473,7 @@
         <v>137</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C54" s="19">
         <v>1</v>
@@ -6461,8 +6485,12 @@
       <c r="F54" s="3">
         <v>1</v>
       </c>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
+      <c r="G54" s="3">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -6473,10 +6501,10 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C55" s="19">
         <v>1</v>
@@ -6496,16 +6524,14 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
-      <c r="O55" s="3">
-        <v>1</v>
-      </c>
+      <c r="O55" s="3"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C56" s="19">
         <v>1</v>
@@ -6525,21 +6551,27 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
+      <c r="O56" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C57" s="19">
         <v>1</v>
       </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -6555,18 +6587,14 @@
         <v>138</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C58" s="19">
         <v>1</v>
       </c>
       <c r="D58" s="3"/>
-      <c r="E58" s="3">
-        <v>1</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1</v>
-      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -6579,10 +6607,10 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C59" s="19">
         <v>1</v>
@@ -6602,16 +6630,14 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
-      <c r="O59" s="3">
-        <v>1</v>
-      </c>
+      <c r="O59" s="3"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C60" s="19">
         <v>1</v>
@@ -6631,21 +6657,27 @@
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
+      <c r="O60" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C61" s="19">
         <v>1</v>
       </c>
       <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1</v>
+      </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -6661,7 +6693,7 @@
         <v>139</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C62" s="19">
         <v>1</v>
@@ -6681,10 +6713,10 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C63" s="19">
         <v>1</v>
@@ -6707,7 +6739,7 @@
         <v>140</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C64" s="19">
         <v>1</v>
@@ -6730,18 +6762,14 @@
         <v>140</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C65" s="19">
         <v>1</v>
       </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="3">
-        <v>1</v>
-      </c>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -6754,17 +6782,21 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C66" s="19">
         <v>1</v>
       </c>
       <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
+      <c r="E66" s="3">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -6780,7 +6812,7 @@
         <v>141</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C67" s="19">
         <v>1</v>
@@ -6803,7 +6835,7 @@
         <v>141</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C68" s="19">
         <v>1</v>
@@ -6826,7 +6858,7 @@
         <v>141</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C69" s="19">
         <v>1</v>
@@ -6849,7 +6881,7 @@
         <v>141</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C70" s="19">
         <v>1</v>
@@ -6872,7 +6904,7 @@
         <v>141</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C71" s="19">
         <v>1</v>
@@ -6892,10 +6924,10 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C72" s="19">
         <v>1</v>
@@ -6918,7 +6950,7 @@
         <v>142</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C73" s="19">
         <v>1</v>
@@ -6930,12 +6962,8 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="3">
-        <v>1</v>
-      </c>
-      <c r="L73" s="3">
-        <v>1</v>
-      </c>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
@@ -6945,7 +6973,7 @@
         <v>142</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C74" s="19">
         <v>1</v>
@@ -6957,18 +6985,22 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
+      <c r="K74" s="3">
+        <v>1</v>
+      </c>
+      <c r="L74" s="3">
+        <v>1</v>
+      </c>
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C75" s="19">
         <v>1</v>
@@ -6991,18 +7023,14 @@
         <v>143</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C76" s="19">
         <v>1</v>
       </c>
       <c r="D76" s="3"/>
-      <c r="E76" s="3">
-        <v>1</v>
-      </c>
-      <c r="F76" s="3">
-        <v>1</v>
-      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -7018,14 +7046,18 @@
         <v>143</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" s="19">
         <v>1</v>
       </c>
       <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1</v>
+      </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -7041,7 +7073,7 @@
         <v>143</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C78" s="19">
         <v>1</v>
@@ -7055,12 +7087,8 @@
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
-      <c r="M78" s="3">
-        <v>1</v>
-      </c>
-      <c r="N78" s="3">
-        <v>1</v>
-      </c>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
       <c r="O78" s="3"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -7068,7 +7096,7 @@
         <v>143</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="19">
         <v>1</v>
@@ -7082,8 +7110,12 @@
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
+      <c r="M79" s="3">
+        <v>1</v>
+      </c>
+      <c r="N79" s="3">
+        <v>1</v>
+      </c>
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -7091,7 +7123,7 @@
         <v>143</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="19">
         <v>1</v>
@@ -7111,29 +7143,21 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C81" s="19">
         <v>1</v>
       </c>
       <c r="D81" s="3"/>
-      <c r="E81" s="3">
-        <v>1</v>
-      </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="3">
-        <v>1</v>
-      </c>
-      <c r="J81" s="3">
-        <v>1</v>
-      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
@@ -7145,7 +7169,7 @@
         <v>144</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C82" s="19">
         <v>1</v>
@@ -7154,17 +7178,19 @@
       <c r="E82" s="3">
         <v>1</v>
       </c>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3">
-        <v>1</v>
-      </c>
-      <c r="L82" s="3">
-        <v>1</v>
-      </c>
+      <c r="I82" s="3">
+        <v>1</v>
+      </c>
+      <c r="J82" s="3">
+        <v>1</v>
+      </c>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
@@ -7174,20 +7200,26 @@
         <v>144</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C83" s="19">
         <v>1</v>
       </c>
       <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+      <c r="E83" s="3">
+        <v>1</v>
+      </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
+      <c r="K83" s="3">
+        <v>1</v>
+      </c>
+      <c r="L83" s="3">
+        <v>1</v>
+      </c>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
@@ -7197,15 +7229,13 @@
         <v>144</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C84" s="19">
         <v>1</v>
       </c>
       <c r="D84" s="3"/>
-      <c r="E84" s="3">
-        <v>1</v>
-      </c>
+      <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -7222,13 +7252,15 @@
         <v>144</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C85" s="19">
         <v>1</v>
       </c>
       <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3">
+        <v>1</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -7245,7 +7277,7 @@
         <v>144</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C86" s="19">
         <v>1</v>
@@ -7268,15 +7300,13 @@
         <v>144</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" s="19">
         <v>1</v>
       </c>
       <c r="D87" s="3"/>
-      <c r="E87" s="3">
-        <v>1</v>
-      </c>
+      <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -7293,13 +7323,15 @@
         <v>144</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C88" s="19">
         <v>1</v>
       </c>
       <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
+      <c r="E88" s="3">
+        <v>1</v>
+      </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -7312,22 +7344,18 @@
       <c r="O88" s="3"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B89" s="24" t="s">
-        <v>76</v>
+      <c r="A89" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B89" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="C89" s="19">
         <v>1</v>
       </c>
       <c r="D89" s="3"/>
-      <c r="E89" s="3">
-        <v>1</v>
-      </c>
-      <c r="F89" s="3">
-        <v>1</v>
-      </c>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -7337,6 +7365,56 @@
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
       <c r="O89" s="3"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C90" s="19">
+        <v>1</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C91" s="19">
+        <v>1</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>1</v>
+      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C21:C22 C2:C19">
@@ -7348,7 +7426,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C89">
+  <conditionalFormatting sqref="C3:C91">
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -7375,7 +7453,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:O89">
+  <conditionalFormatting sqref="D3:O91">
     <cfRule type="iconSet" priority="17">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>